<commit_message>
feat(assets): update attachments (#852)
</commit_message>
<xml_diff>
--- a/src/main/assets/files/pre-editing-request-form.xlsx
+++ b/src/main/assets/files/pre-editing-request-form.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8E9B67D-C90F-4F6C-A8A5-BD0CE0A052CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://justiceuk-my.sharepoint.com/personal/colin_clixby_justice_gov_uk/Documents/Documents/#01 DTS Video Product Team/PRE/Editing/Forms/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="190" documentId="8_{BC79492A-3608-458B-BC29-AB251F64BBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E703B68E-677A-4517-8777-A19AC202DA31}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="19905" windowHeight="17925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31110" yWindow="1845" windowWidth="25440" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quick Guide" sheetId="2" r:id="rId1"/>
@@ -14,10 +19,10 @@
     <sheet name="PRE Service Team Only" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Court inboxes'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Court inboxes'!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Editing Form'!$B$37:$H$38</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="198">
   <si>
     <t xml:space="preserve">Quick Guide – Making edits to a recording </t>
   </si>
@@ -271,9 +276,6 @@
     <t>PRE.edits.KingstonCC@justice.gov.uk</t>
   </si>
   <si>
-    <t>Leeds Combined Court Centre</t>
-  </si>
-  <si>
     <t>PRE.edits.LeedsCC@justice.gov.uk</t>
   </si>
   <si>
@@ -337,7 +339,406 @@
     <t>PRE.Edits.ExeterCC@justice.gov.uk</t>
   </si>
   <si>
-    <t>V2.3</t>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>North East</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>North West</t>
+  </si>
+  <si>
+    <t>South East</t>
+  </si>
+  <si>
+    <t>Midlands</t>
+  </si>
+  <si>
+    <t>South West</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
+    <t>PRE.Edits.PlymouthCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.BournemouthCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.SouthamptonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Bristol Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.BristolCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.PortsmouthCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.SwindonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.WinchesterCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.SalisburyCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.TruroCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Gloucester Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.GloucesterCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.TauntonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Chelmsford Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.ChelmsfordCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Ipswich Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.IpswichCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.BasildonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.NorwichCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Maidstone Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.MaidstoneCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.CanterburyCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Aylesbury Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.AylesburyCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.OxfordCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Cambridge Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.CambridgeCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Luton Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.LutonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>St Albans Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.StAlbansCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Guildford Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.GuildfordCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.LewesCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Chester Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.ChesterCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.CarlisleCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.MCRCrownSqCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.MCRMinshullStCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Bolton Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.BoltonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.PrestonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Bradford Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.BradfordCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>York Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.YorkCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Newcastle Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.NewcastleCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.SheffieldCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.GrimsbyCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.HullCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Croydon Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.CroydonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Inner London Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.InnerLondonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Woolwich Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.WoolwichCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Southwark Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.SouthwarkCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Wood Green Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.WoodGreenCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Central Criminal Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.CentralCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Snaresbrook Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.SnaresbrookCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Isleworth Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.IsleworthCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Cardiff Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.CardiffCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.MerthyrCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Swansea Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.SwanseaCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Shrewsbury Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.ShrewsburyCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.StaffordCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.StokeCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.WorcesterCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Birmingham Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.BirminghamCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.WolverhamptonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.WarwickCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Lincoln Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.LincolnCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Leicester Crown Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.LeicesterCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.NorthamptonCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Basildon Combined Court</t>
+  </si>
+  <si>
+    <t>Bournemouth Combined Court</t>
+  </si>
+  <si>
+    <t>Canterbury Combined Court</t>
+  </si>
+  <si>
+    <t>Carlisle Combined Court</t>
+  </si>
+  <si>
+    <t>Derby Combined Court</t>
+  </si>
+  <si>
+    <t>Great Grimsby Combined Court</t>
+  </si>
+  <si>
+    <t>Harrow Crown Court</t>
+  </si>
+  <si>
+    <t>Kingston-upon-Hull Combined Court</t>
+  </si>
+  <si>
+    <t>Isle of Wight Combined Court</t>
+  </si>
+  <si>
+    <t>Leeds Combined Court</t>
+  </si>
+  <si>
+    <t>Lewes Combined Court</t>
+  </si>
+  <si>
+    <t>Manchester Crown Court</t>
+  </si>
+  <si>
+    <t>Manchester Minshull Street Crown Court</t>
+  </si>
+  <si>
+    <t>Merthyr Tydfil  Combined Court</t>
+  </si>
+  <si>
+    <t>Northampton Combined Court</t>
+  </si>
+  <si>
+    <t>Norwich Combined Court</t>
+  </si>
+  <si>
+    <t>Oxford Combined Court</t>
+  </si>
+  <si>
+    <t>Plymouth Combined Court</t>
+  </si>
+  <si>
+    <t>Portsmouth Combined Court</t>
+  </si>
+  <si>
+    <t>Preston Combined Court</t>
+  </si>
+  <si>
+    <t>Salisbury Law Courts</t>
+  </si>
+  <si>
+    <t>Sheffield Combined Court</t>
+  </si>
+  <si>
+    <t>Southampton Combined Court</t>
+  </si>
+  <si>
+    <t>Stafford Combined Court</t>
+  </si>
+  <si>
+    <t>Stoke-on-Trent Combined Court</t>
+  </si>
+  <si>
+    <t>Swindon Combined Court</t>
+  </si>
+  <si>
+    <t>Taunton Combined Court</t>
+  </si>
+  <si>
+    <t>Teesside Combined Court</t>
+  </si>
+  <si>
+    <t>Truro Combined Court</t>
+  </si>
+  <si>
+    <t>Warwick Combined Court</t>
+  </si>
+  <si>
+    <t>Winchester Combined Court</t>
+  </si>
+  <si>
+    <t>Wolverhampton Combined Court</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worcester Combined Court </t>
+  </si>
+  <si>
+    <t>S28-LeedsMC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Leeds Youth Court</t>
+  </si>
+  <si>
+    <t>PRE.Edits.DerbyCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.HarrowCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.NewportIOWCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>PRE.Edits.TeessideCC@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>V3.1</t>
   </si>
 </sst>
 </file>
@@ -555,7 +956,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -999,23 +1400,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1149,7 +1539,6 @@
     <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1362,63 +1751,52 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>790682</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="HM Courts &amp; Tribunals Service">
+        <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED1EE88E-D7E2-43E8-B741-D53266AEC701}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73DA6F37-C73E-7BF0-981E-B407F9CF885B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="66675" y="85725"/>
-          <a:ext cx="2571750" cy="819150"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9974096" cy="998483"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1726,7 +2104,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:N27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1734,38 +2112,38 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="55"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
     </row>
     <row r="4" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="61"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="60"/>
     </row>
     <row r="5" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
@@ -1783,38 +2161,38 @@
       <c r="N5" s="17"/>
     </row>
     <row r="6" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="52"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="51"/>
     </row>
     <row r="7" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="52"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
     </row>
     <row r="8" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
@@ -1832,38 +2210,38 @@
       <c r="N8" s="19"/>
     </row>
     <row r="9" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="52"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="51"/>
     </row>
     <row r="10" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="52"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="51"/>
     </row>
     <row r="11" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
@@ -1884,37 +2262,37 @@
       <c r="B12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="52"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="51"/>
     </row>
     <row r="13" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="52"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="51"/>
     </row>
     <row r="14" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
@@ -1935,54 +2313,54 @@
       <c r="B15" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="52"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="51"/>
     </row>
     <row r="16" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18"/>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="52"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="51"/>
     </row>
     <row r="17" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="52"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="51"/>
     </row>
     <row r="18" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
@@ -2000,21 +2378,21 @@
       <c r="N18" s="19"/>
     </row>
     <row r="19" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="52"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="51"/>
     </row>
     <row r="20" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="18"/>
@@ -2032,21 +2410,21 @@
       <c r="N20" s="19"/>
     </row>
     <row r="21" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="58"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="57"/>
     </row>
     <row r="22" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="18"/>
@@ -2064,21 +2442,21 @@
       <c r="N22" s="19"/>
     </row>
     <row r="23" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="52"/>
+      <c r="B23" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="51"/>
     </row>
     <row r="24" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="18"/>
@@ -2096,38 +2474,38 @@
       <c r="N24" s="19"/>
     </row>
     <row r="25" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="52"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="51"/>
     </row>
     <row r="26" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="52"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="51"/>
     </row>
     <row r="27" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
@@ -2143,11 +2521,11 @@
       <c r="L27" s="22"/>
       <c r="M27" s="22"/>
       <c r="N27" s="48" t="s">
-        <v>65</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ugOFX8Sp+tfkNy66Af08AKk4Tbm3Gw356uGnyG6/z6DGsRvt3tasWmYh8JoiQBFxdnyGZ4jNh9liujTLAhqeCw==" saltValue="HSp88reEz96LBkxrZxu3fA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="OankUjCsHSgvU98py53LqNXhLU/uc3IYnQ8Xs2fMkPdJI/NFetXWceBgtg2Q0tOr7+lNGrV4ujv9ADWvDiKO6Q==" saltValue="ldMhVUzfOQLRg5AoXfPv1g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="16">
     <mergeCell ref="B23:N23"/>
     <mergeCell ref="B25:N25"/>
@@ -2176,8 +2554,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,7 +2599,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2232,7 +2610,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2245,16 +2623,16 @@
     </row>
     <row r="6" spans="1:9" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="64"/>
+      <c r="B6" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
@@ -2268,16 +2646,16 @@
     </row>
     <row r="8" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="85"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="84"/>
     </row>
     <row r="9" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -2330,16 +2708,16 @@
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="78"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -2355,12 +2733,12 @@
       <c r="E13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="86" t="s">
+      <c r="F13" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="78"/>
     </row>
     <row r="14" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
@@ -2373,10 +2751,10 @@
         <f t="shared" ref="E14:E28" si="0">IF(D14-C14=0,"",D14-C14)</f>
         <v/>
       </c>
-      <c r="F14" s="80"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="82"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="81"/>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
@@ -2389,10 +2767,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F15" s="80"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="82"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="81"/>
     </row>
     <row r="16" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
@@ -2405,10 +2783,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F16" s="80"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="82"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="81"/>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
@@ -2421,10 +2799,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="82"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="81"/>
     </row>
     <row r="18" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
@@ -2437,10 +2815,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F18" s="80"/>
-      <c r="G18" s="81"/>
-      <c r="H18" s="81"/>
-      <c r="I18" s="82"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="81"/>
     </row>
     <row r="19" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
@@ -2453,10 +2831,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F19" s="80"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="82"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="81"/>
     </row>
     <row r="20" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
@@ -2469,10 +2847,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F20" s="80"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
-      <c r="I20" s="82"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="81"/>
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
@@ -2485,10 +2863,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F21" s="80"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="82"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="81"/>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
@@ -2501,10 +2879,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F22" s="80"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="82"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="81"/>
     </row>
     <row r="23" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
@@ -2517,10 +2895,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F23" s="80"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
-      <c r="I23" s="82"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="81"/>
     </row>
     <row r="24" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
@@ -2533,10 +2911,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F24" s="80"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="81"/>
-      <c r="I24" s="82"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="81"/>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
@@ -2549,10 +2927,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="82"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="81"/>
     </row>
     <row r="26" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
@@ -2565,10 +2943,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F26" s="80"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="81"/>
-      <c r="I26" s="82"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="81"/>
     </row>
     <row r="27" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
@@ -2581,10 +2959,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F27" s="80"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="81"/>
-      <c r="I27" s="82"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="81"/>
     </row>
     <row r="28" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
@@ -2597,23 +2975,23 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F28" s="80"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="82"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="81"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="74" t="s">
+      <c r="B29" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="76"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="75"/>
     </row>
     <row r="30" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -2628,54 +3006,54 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="76"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="75"/>
     </row>
     <row r="32" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="73"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="72"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="67"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="66"/>
     </row>
     <row r="34" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
-      <c r="B34" s="68" t="str">
-        <f>IFERROR(HYPERLINK("mailto:" &amp; VLOOKUP(B10,'Court inboxes'!A2:B1000,2,FALSE),VLOOKUP(B10,'Court inboxes'!A2:B1000,2,FALSE)),"")</f>
+      <c r="B34" s="67" t="str">
+        <f>IFERROR(HYPERLINK("mailto:" &amp; VLOOKUP(B10,'Court inboxes'!B2:C991,2,FALSE),VLOOKUP(B10,'Court inboxes'!B2:C991,2,FALSE)),"")</f>
         <v/>
       </c>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="70"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="69"/>
     </row>
     <row r="35" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
@@ -2689,71 +3067,71 @@
     </row>
     <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
-      <c r="B36" s="97" t="s">
+      <c r="B36" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="98"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="99"/>
+      <c r="C36" s="97"/>
+      <c r="D36" s="97"/>
+      <c r="E36" s="97"/>
+      <c r="F36" s="97"/>
+      <c r="G36" s="97"/>
+      <c r="H36" s="97"/>
+      <c r="I36" s="98"/>
     </row>
     <row r="37" spans="1:9" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="100" t="s">
+      <c r="B37" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="94"/>
+      <c r="C37" s="93"/>
       <c r="D37" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="93" t="s">
+      <c r="E37" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="94"/>
-      <c r="G37" s="93" t="s">
+      <c r="F37" s="93"/>
+      <c r="G37" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="H37" s="102"/>
-      <c r="I37" s="103"/>
+      <c r="H37" s="101"/>
+      <c r="I37" s="102"/>
     </row>
     <row r="38" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="101"/>
-      <c r="C38" s="96"/>
+      <c r="B38" s="100"/>
+      <c r="C38" s="95"/>
       <c r="D38" s="35"/>
-      <c r="E38" s="95"/>
-      <c r="F38" s="96"/>
-      <c r="G38" s="90"/>
-      <c r="H38" s="91"/>
-      <c r="I38" s="92"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="95"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="90"/>
+      <c r="I38" s="91"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="67"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="66"/>
     </row>
     <row r="40" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
-      <c r="B40" s="87" t="s">
+      <c r="B40" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="88"/>
-      <c r="D40" s="88"/>
-      <c r="E40" s="88"/>
-      <c r="F40" s="88"/>
-      <c r="G40" s="88"/>
-      <c r="H40" s="88"/>
-      <c r="I40" s="89"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="87"/>
+      <c r="I40" s="88"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
@@ -2765,7 +3143,7 @@
       <c r="H41" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="TCnA+zOTtn9fDshsWbgt3ahaBQfUBBejiH6iwD73iWlKWPjBp/pi2XLT8g5wsJximyeBL+AmqRRhdjHkvQGvIQ==" saltValue="e8KkCBcgyFW8xoki46QuXA==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZJl6C0+3RSif1cChrGH+ZCArCcNy8FgFRMR8TJ4hM8nKRIHNUwv8TzH+dCUIYEFexirKXbPZIZHIEGvWT2Q6UA==" saltValue="1QgChSU61xh8PkwkYxWw3Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0"/>
   <protectedRanges>
     <protectedRange sqref="B32" name="Range6"/>
     <protectedRange sqref="I10 B10:H11" name="Range2"/>
@@ -2848,7 +3226,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Name" error="This is not a valid Court" promptTitle="Court Name" prompt="Please select the court where the recording was made from the drop down list" xr:uid="{489ADCB8-0B89-419D-B903-DB0BFBE3CA28}">
           <x14:formula1>
-            <xm:f>'Court inboxes'!$A$2:$A$1000</xm:f>
+            <xm:f>'Court inboxes'!$B$2:$B$991</xm:f>
           </x14:formula1>
           <xm:sqref>B10</xm:sqref>
         </x14:dataValidation>
@@ -2861,96 +3239,801 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF3F12E-E37B-4459-B87E-A2B329987312}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="C1" s="40" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="C18" s="41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="41" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="C29" s="41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="41" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="41" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="C35" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="41" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="41" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="C41" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="41" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="41" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="41" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="41" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="C50" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="49" t="s">
-        <v>56</v>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="41" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" s="41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="C59" s="41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="C62" s="41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" s="41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C66" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="C67" s="41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C69" s="41" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="C70" s="41" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C71" s="41" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{9AF3F12E-E37B-4459-B87E-A2B329987312}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B9">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <sheetProtection algorithmName="SHA-512" hashValue="0GTOrtQvKdTW33/e/rvmVo+x9ujHTM8M9SY0bqHK6BK+wU6/ykI6+6xiDJL/97K8XrNHw7Wml873sGEETh5UjQ==" saltValue="1F76tK+fEiWpDeEVxpfEsA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <autoFilter ref="A1:C1" xr:uid="{9AF3F12E-E37B-4459-B87E-A2B329987312}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2971,41 +4054,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="106" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="108"/>
+    </row>
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="109"/>
-    </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="106"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="105"/>
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="45"/>
       <c r="C3" s="46"/>
@@ -3021,7 +4104,7 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="44"/>
@@ -3035,7 +4118,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="44"/>
@@ -3049,7 +4132,7 @@
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="44"/>
@@ -3063,24 +4146,24 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="24"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="24"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4gUNfODPbu27qkWnC442RQ1zgQ/RrF4IHmgHGflk2wQfX5EoaABsutkrWMrWPU4y9kaVq3WcntZfUyQTfgc+ng==" saltValue="pXZZQzUz0GDd2pguntnDEg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TJq+N6mE4n/D1obBFK1nZWvFbKLqLnij1U6Ev5lBgU8lJFdxIUiSm1yTOC/J2zYSoz3lq9M30KnpDK40yWflmQ==" saltValue="ahLYc4JG49KM1Be02KF63g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
@@ -3091,26 +4174,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="d20a315a-b416-49e1-9bd6-0d2a939cd722" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100729551BC3DBA0747ADE92B04040EF5B7" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d94158b32b66a28d0b525110423b84fb">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d20a315a-b416-49e1-9bd6-0d2a939cd722" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="32ae12ca1fab071fbac7569c1e65da70" ns2:_="">
-    <xsd:import namespace="d20a315a-b416-49e1-9bd6-0d2a939cd722"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EA8326E2BA23A479A860402065EE35A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dd581be8521772c4187600b7a4899808">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e14a74be-12ac-4ba0-804e-2186ac14cf4c" xmlns:ns3="001afb37-2a5c-4754-b688-99e7a82a5888" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea890d7776cad9d004aa10e721fb1d02" ns2:_="" ns3:_="">
+    <xsd:import namespace="e14a74be-12ac-4ba0-804e-2186ac14cf4c"/>
+    <xsd:import namespace="001afb37-2a5c-4754-b688-99e7a82a5888"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -3119,9 +4186,18 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3129,7 +4205,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d20a315a-b416-49e1-9bd6-0d2a939cd722" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e14a74be-12ac-4ba0-804e-2186ac14cf4c" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -3142,20 +4218,95 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="13" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="95b7e4bc-7c04-4239-a3c8-056ff7db7bf8" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="17" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="21" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="22" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="001afb37-2a5c-4754-b688-99e7a82a5888" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{38f8756e-469a-46d6-8af2-7d59e75d5fc1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="001afb37-2a5c-4754-b688-99e7a82a5888">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -3257,44 +4408,51 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="e14a74be-12ac-4ba0-804e-2186ac14cf4c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e14a74be-12ac-4ba0-804e-2186ac14cf4c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="001afb37-2a5c-4754-b688-99e7a82a5888" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42B16326-312F-41AC-B67D-C1D6EF3BD024}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B82F41E1-8A98-46EC-9064-2F56AEB1E246}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d20a315a-b416-49e1-9bd6-0d2a939cd722"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d20a315a-b416-49e1-9bd6-0d2a939cd722"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EDD2F1A-4C13-421F-8DB6-52A2730C1658}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04B5EC0B-DFF6-4046-A1C6-E8B2BD1B77B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d20a315a-b416-49e1-9bd6-0d2a939cd722"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>